<commit_message>
fix and update constraints
</commit_message>
<xml_diff>
--- a/assignment_problem/output.xlsx
+++ b/assignment_problem/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>teacher</t>
   </si>
@@ -32,19 +32,37 @@
     <t>x</t>
   </si>
   <si>
+    <t>Gomory</t>
+  </si>
+  <si>
+    <t>Benders</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
     <t>Dantzig</t>
   </si>
   <si>
     <t>Wolfe</t>
   </si>
   <si>
-    <t>Gomory</t>
-  </si>
-  <si>
-    <t>Benders</t>
-  </si>
-  <si>
-    <t>Dijkstra</t>
+    <t>Matteo</t>
+  </si>
+  <si>
+    <t>Cata</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Tomás</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Manuel</t>
   </si>
   <si>
     <t>Ricardo</t>
@@ -53,37 +71,22 @@
     <t>Juan</t>
   </si>
   <si>
-    <t>Matteo</t>
-  </si>
-  <si>
-    <t>Tomás</t>
-  </si>
-  <si>
-    <t>Jaime</t>
-  </si>
-  <si>
-    <t>Cata</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Manuel</t>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
   </si>
   <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>index</t>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Thursday</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
         <v>18</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -483,16 +486,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -503,10 +506,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -520,13 +523,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -537,13 +540,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -551,16 +554,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -568,16 +571,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -588,13 +591,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -602,16 +605,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -625,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D11">
         <v>18</v>
@@ -642,10 +645,10 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -658,249 +661,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>15</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
         <v>19</v>
       </c>
-      <c r="E3">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <v>18</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>18</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
-        <v>18</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10">
-        <v>18</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12">
+      <c r="C2">
         <v>1</v>
       </c>
     </row>

</xml_diff>